<commit_message>
Update sample bank and book Excel data
</commit_message>
<xml_diff>
--- a/data_samples/bank_statement_example.xlsx
+++ b/data_samples/bank_statement_example.xlsx
@@ -1,20 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28014"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\untun\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45782D6A-E43F-435E-9A39-ED0AF9479C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -101,16 +119,22 @@
   </si>
   <si>
     <t>FEE-002</t>
+  </si>
+  <si>
+    <t>debit</t>
+  </si>
+  <si>
+    <t>credit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,29 +182,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -218,7 +264,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -252,6 +298,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -286,9 +333,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,14 +509,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,13 +533,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -490,13 +553,20 @@
         <v>4</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>1500000</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="F2">
+        <f>D2-C2</f>
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45658</v>
       </c>
@@ -504,13 +574,20 @@
         <v>5</v>
       </c>
       <c r="C3">
+        <v>5000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F14" si="0">D3-C3</f>
         <v>-5000</v>
       </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45659</v>
       </c>
@@ -518,13 +595,20 @@
         <v>6</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>2500000</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45659</v>
       </c>
@@ -532,13 +616,20 @@
         <v>7</v>
       </c>
       <c r="C5">
+        <v>1000000</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
         <v>-1000000</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45660</v>
       </c>
@@ -546,13 +637,20 @@
         <v>8</v>
       </c>
       <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <v>1750000</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1750000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45661</v>
       </c>
@@ -560,13 +658,20 @@
         <v>9</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>2000000</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45661</v>
       </c>
@@ -574,13 +679,20 @@
         <v>10</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>25000</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45662</v>
       </c>
@@ -588,13 +700,20 @@
         <v>11</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>3000000</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45663</v>
       </c>
@@ -602,13 +721,20 @@
         <v>12</v>
       </c>
       <c r="C10">
+        <v>1200000</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
         <v>-1200000</v>
       </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45664</v>
       </c>
@@ -616,13 +742,20 @@
         <v>13</v>
       </c>
       <c r="C11">
+        <v>850000</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
         <v>-850000</v>
       </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45665</v>
       </c>
@@ -630,13 +763,20 @@
         <v>14</v>
       </c>
       <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
         <v>2200000</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2200000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45666</v>
       </c>
@@ -644,13 +784,20 @@
         <v>15</v>
       </c>
       <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
         <v>1800000</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45667</v>
       </c>
@@ -658,10 +805,17 @@
         <v>5</v>
       </c>
       <c r="C14">
+        <v>7500</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
         <v>-7500</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>